<commit_message>
Tela de login, e ajustes nos bancos de dados realizado
</commit_message>
<xml_diff>
--- a/academia_app/base/treinos.xlsx
+++ b/academia_app/base/treinos.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/607c4759856959e0/Documentos/_repositorios_/Projetos/02_academia_app/academia_app/base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{232220E7-6469-4400-8F27-A04433DD145F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0260D949-5701-4FF3-A504-1CDEAB042C0B}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="8_{232220E7-6469-4400-8F27-A04433DD145F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{09561F02-534F-4C25-BF05-BE301E3FD861}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{D834B919-9E85-4F8F-893C-9AAA66FB1811}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{D834B919-9E85-4F8F-893C-9AAA66FB1811}"/>
   </bookViews>
   <sheets>
-    <sheet name="Treino A" sheetId="1" r:id="rId1"/>
+    <sheet name="Treinos" sheetId="1" r:id="rId1"/>
+    <sheet name="Base" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="24">
   <si>
     <t>Treino A</t>
   </si>
@@ -53,60 +54,36 @@
     <t>Pulley Frente</t>
   </si>
   <si>
-    <t>local/Pulley_Frente.png</t>
-  </si>
-  <si>
     <t>Costas</t>
   </si>
   <si>
     <t>Remada Articulada Pronada</t>
   </si>
   <si>
-    <t>local/Remada_Articulada_Pronada.png</t>
-  </si>
-  <si>
     <t>Remada Cavalinho</t>
   </si>
   <si>
-    <t>local/Remada_Cavalinho.png</t>
-  </si>
-  <si>
     <t>Pull Down</t>
   </si>
   <si>
-    <t>local/Pull_Down.png</t>
-  </si>
-  <si>
     <t>Rosca Direta com Barra W</t>
   </si>
   <si>
-    <t>local/Rosca_Direta_Bar_W.png</t>
-  </si>
-  <si>
     <t>Bíceps</t>
   </si>
   <si>
     <t>Rosca Alternada</t>
   </si>
   <si>
-    <t>local/Rosca_Alternada.png</t>
-  </si>
-  <si>
     <t>Rosca Inversa com Barra W</t>
   </si>
   <si>
-    <t>local/Rosca_Inversa_Bar_W.png</t>
-  </si>
-  <si>
     <t>Antebraço</t>
   </si>
   <si>
     <t>Abdominal Remador</t>
   </si>
   <si>
-    <t>local/Abdominal_Remador.png</t>
-  </si>
-  <si>
     <t>Abdominais</t>
   </si>
   <si>
@@ -114,6 +91,24 @@
   </si>
   <si>
     <t>Treino</t>
+  </si>
+  <si>
+    <t>Treino B</t>
+  </si>
+  <si>
+    <t>Voador / Peck Deck</t>
+  </si>
+  <si>
+    <t>Supino Reto com Halter</t>
+  </si>
+  <si>
+    <t>Supino Inclinado com  Halter</t>
+  </si>
+  <si>
+    <t>Crucifixo no Cross Over</t>
+  </si>
+  <si>
+    <t>Peito</t>
   </si>
 </sst>
 </file>
@@ -142,12 +137,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -162,12 +163,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -508,27 +512,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{172E9C2E-4188-4DBB-9D62-6E3F04F3AFE2}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="40.85546875" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -540,7 +544,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -548,135 +552,1121 @@
         <v>4</v>
       </c>
       <c r="C2" s="2">
+        <f>VLOOKUP(B2,Base!A:D,2,FALSE)</f>
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="69" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="str">
+        <f>VLOOKUP(C2,Base!B:E,2,FALSE)</f>
+        <v>local/Pulley_Frente.png</v>
+      </c>
+      <c r="E2" s="2" t="str">
+        <f>VLOOKUP(D2,Base!C:F,2,FALSE)</f>
+        <v>Costas</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2">
+        <f>VLOOKUP(B3,Base!A:D,2,FALSE)</f>
         <v>2</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="D3" s="2" t="str">
+        <f>VLOOKUP(C3,Base!B:E,2,FALSE)</f>
+        <v>local/Remada_Articulada_Pronada.png</v>
+      </c>
+      <c r="E3" s="2" t="str">
+        <f>VLOOKUP(D3,Base!C:F,2,FALSE)</f>
+        <v>Costas</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" s="2">
+        <f>VLOOKUP(B4,Base!A:D,2,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="str">
+        <f>VLOOKUP(C4,Base!B:E,2,FALSE)</f>
+        <v>local/Remada_Cavalinho.png</v>
+      </c>
+      <c r="E4" s="2" t="str">
+        <f>VLOOKUP(D4,Base!C:F,2,FALSE)</f>
+        <v>Costas</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2">
+        <f>VLOOKUP(B5,Base!A:D,2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="D5" s="2" t="str">
+        <f>VLOOKUP(C5,Base!B:E,2,FALSE)</f>
+        <v>local/Pull_Down.png</v>
+      </c>
+      <c r="E5" s="2" t="str">
+        <f>VLOOKUP(D5,Base!C:F,2,FALSE)</f>
+        <v>Costas</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2">
+        <f>VLOOKUP(B6,Base!A:D,2,FALSE)</f>
         <v>5</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="D6" s="2" t="str">
+        <f>VLOOKUP(C6,Base!B:E,2,FALSE)</f>
+        <v>local/Rosca_Direta_com_Barra_W.png</v>
+      </c>
+      <c r="E6" s="2" t="str">
+        <f>VLOOKUP(D6,Base!C:F,2,FALSE)</f>
+        <v>Bíceps</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2">
+        <f>VLOOKUP(B7,Base!A:D,2,FALSE)</f>
         <v>6</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="51.75" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="str">
+        <f>VLOOKUP(C7,Base!B:E,2,FALSE)</f>
+        <v>local/Rosca_Alternada.png</v>
+      </c>
+      <c r="E7" s="2" t="str">
+        <f>VLOOKUP(D7,Base!C:F,2,FALSE)</f>
+        <v>Bíceps</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C8" s="2">
+        <f>VLOOKUP(B8,Base!A:D,2,FALSE)</f>
         <v>7</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="69" x14ac:dyDescent="0.25">
+      <c r="D8" s="2" t="str">
+        <f>VLOOKUP(C8,Base!B:E,2,FALSE)</f>
+        <v>local/Rosca_Inversa_com_Barra_W.png</v>
+      </c>
+      <c r="E8" s="2" t="str">
+        <f>VLOOKUP(D8,Base!C:F,2,FALSE)</f>
+        <v>Antebraço</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2">
+        <f>VLOOKUP(B9,Base!A:D,2,FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="str">
+        <f>VLOOKUP(C9,Base!B:E,2,FALSE)</f>
+        <v>local/Abdominal_Remador.png</v>
+      </c>
+      <c r="E9" s="2" t="str">
+        <f>VLOOKUP(D9,Base!C:F,2,FALSE)</f>
+        <v>Abdominais</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2">
+        <f>VLOOKUP(B10,Base!A:D,2,FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="D10" s="2" t="str">
+        <f>VLOOKUP(C10,Base!B:E,2,FALSE)</f>
+        <v>local/Supino_Reto_com_Halter.png</v>
+      </c>
+      <c r="E10" s="2" t="str">
+        <f>VLOOKUP(D10,Base!C:F,2,FALSE)</f>
+        <v>Peito</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="2">
-        <v>8</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="C11" s="2">
+        <f>VLOOKUP(B11,Base!A:D,2,FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="D11" s="2" t="str">
+        <f>VLOOKUP(C11,Base!B:E,2,FALSE)</f>
+        <v>local/Supino_Inclinado_com__Halter.png</v>
+      </c>
+      <c r="E11" s="2" t="str">
+        <f>VLOOKUP(D11,Base!C:F,2,FALSE)</f>
+        <v>Peito</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="34.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>23</v>
+      <c r="C12" s="2">
+        <f>VLOOKUP(B12,Base!A:D,2,FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="D12" s="2" t="str">
+        <f>VLOOKUP(C12,Base!B:E,2,FALSE)</f>
+        <v>local/Crucifixo_no_Cross_Over.png</v>
+      </c>
+      <c r="E12" s="2" t="str">
+        <f>VLOOKUP(D12,Base!C:F,2,FALSE)</f>
+        <v>Peito</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6124B3D7-6BE7-44DE-AAE7-DF9EB59173DA}">
+  <dimension ref="A1:F89"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11:A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" customWidth="1"/>
+    <col min="4" max="4" width="43.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="str">
+        <f>SUBSTITUTE(CONCATENATE("local/",A2, ".png"), " ","_")</f>
+        <v>local/Pulley_Frente.png</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="str">
+        <f t="shared" ref="C3:C8" si="0">SUBSTITUTE(CONCATENATE("local/",A3, ".png"), " ","_")</f>
+        <v>local/Remada_Articulada_Pronada.png</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>local/Remada_Cavalinho.png</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>local/Pull_Down.png</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>local/Rosca_Direta_com_Barra_W.png</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>local/Rosca_Alternada.png</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>local/Rosca_Inversa_com_Barra_W.png</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="str">
+        <f>SUBSTITUTE(CONCATENATE("local/",A9, ".png"), " ","_")</f>
+        <v>local/Abdominal_Remador.png</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="2">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="str">
+        <f>SUBSTITUTE(CONCATENATE("local/",A10, ".png"), " ","_")</f>
+        <v>local/Voador_/_Peck_Deck.png</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
+      <c r="C11" s="2" t="str">
+        <f>SUBSTITUTE(CONCATENATE("local/",A11, ".png"), " ","_")</f>
+        <v>local/Supino_Reto_com_Halter.png</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="2">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2" t="str">
+        <f>SUBSTITUTE(CONCATENATE("local/",A12, ".png"), " ","_")</f>
+        <v>local/Supino_Inclinado_com__Halter.png</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="2">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="str">
+        <f>SUBSTITUTE(CONCATENATE("local/",A13, ".png"), " ","_")</f>
+        <v>local/Crucifixo_no_Cross_Over.png</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
+        <v>13</v>
+      </c>
+      <c r="C14" s="2" t="str">
+        <f t="shared" ref="C14:C77" si="1">SUBSTITUTE(CONCATENATE("local/",A14, ".png"), " ","_")</f>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
+        <v>14</v>
+      </c>
+      <c r="C15" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
+        <v>17</v>
+      </c>
+      <c r="C18" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <v>18</v>
+      </c>
+      <c r="C19" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
+        <v>19</v>
+      </c>
+      <c r="C20" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <v>20</v>
+      </c>
+      <c r="C21" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B22" s="2">
+        <v>21</v>
+      </c>
+      <c r="C22" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B23" s="2">
+        <v>22</v>
+      </c>
+      <c r="C23" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B24" s="2">
+        <v>23</v>
+      </c>
+      <c r="C24" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B25" s="2">
+        <v>24</v>
+      </c>
+      <c r="C25" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B26" s="2">
+        <v>25</v>
+      </c>
+      <c r="C26" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B27" s="2">
+        <v>26</v>
+      </c>
+      <c r="C27" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B28" s="2">
+        <v>27</v>
+      </c>
+      <c r="C28" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B29" s="2">
+        <v>28</v>
+      </c>
+      <c r="C29" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B30" s="2">
+        <v>29</v>
+      </c>
+      <c r="C30" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B31" s="2">
+        <v>30</v>
+      </c>
+      <c r="C31" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B32" s="2">
+        <v>31</v>
+      </c>
+      <c r="C32" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B33" s="2">
+        <v>32</v>
+      </c>
+      <c r="C33" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B34" s="2">
+        <v>33</v>
+      </c>
+      <c r="C34" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B35" s="2">
+        <v>34</v>
+      </c>
+      <c r="C35" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B36" s="2">
+        <v>35</v>
+      </c>
+      <c r="C36" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B37" s="2">
+        <v>36</v>
+      </c>
+      <c r="C37" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B38" s="2">
+        <v>37</v>
+      </c>
+      <c r="C38" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B39" s="2">
+        <v>38</v>
+      </c>
+      <c r="C39" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B40" s="2">
+        <v>39</v>
+      </c>
+      <c r="C40" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B41" s="2">
+        <v>40</v>
+      </c>
+      <c r="C41" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B42" s="2">
+        <v>41</v>
+      </c>
+      <c r="C42" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B43" s="2">
+        <v>42</v>
+      </c>
+      <c r="C43" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B44" s="2">
+        <v>43</v>
+      </c>
+      <c r="C44" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B45" s="2">
+        <v>44</v>
+      </c>
+      <c r="C45" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B46" s="2">
+        <v>45</v>
+      </c>
+      <c r="C46" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B47" s="2">
+        <v>46</v>
+      </c>
+      <c r="C47" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B48" s="2">
+        <v>47</v>
+      </c>
+      <c r="C48" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B49" s="2">
+        <v>48</v>
+      </c>
+      <c r="C49" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B50" s="2">
+        <v>49</v>
+      </c>
+      <c r="C50" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B51" s="2">
+        <v>50</v>
+      </c>
+      <c r="C51" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B52" s="2">
+        <v>51</v>
+      </c>
+      <c r="C52" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B53" s="2">
+        <v>52</v>
+      </c>
+      <c r="C53" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B54" s="2">
+        <v>53</v>
+      </c>
+      <c r="C54" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B55" s="2">
+        <v>54</v>
+      </c>
+      <c r="C55" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B56" s="2">
+        <v>55</v>
+      </c>
+      <c r="C56" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B57" s="2">
+        <v>56</v>
+      </c>
+      <c r="C57" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B58" s="2">
+        <v>57</v>
+      </c>
+      <c r="C58" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B59" s="2">
+        <v>58</v>
+      </c>
+      <c r="C59" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B60" s="2">
+        <v>59</v>
+      </c>
+      <c r="C60" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B61" s="2">
+        <v>60</v>
+      </c>
+      <c r="C61" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B62" s="2">
+        <v>61</v>
+      </c>
+      <c r="C62" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B63" s="2">
+        <v>62</v>
+      </c>
+      <c r="C63" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B64" s="2">
+        <v>63</v>
+      </c>
+      <c r="C64" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B65" s="2">
+        <v>64</v>
+      </c>
+      <c r="C65" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B66" s="2">
+        <v>65</v>
+      </c>
+      <c r="C66" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B67" s="2">
+        <v>66</v>
+      </c>
+      <c r="C67" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B68" s="2">
+        <v>67</v>
+      </c>
+      <c r="C68" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B69" s="2">
+        <v>68</v>
+      </c>
+      <c r="C69" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B70" s="2">
+        <v>69</v>
+      </c>
+      <c r="C70" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B71" s="2">
+        <v>70</v>
+      </c>
+      <c r="C71" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B72" s="2">
+        <v>71</v>
+      </c>
+      <c r="C72" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B73" s="2">
+        <v>72</v>
+      </c>
+      <c r="C73" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B74" s="2">
+        <v>73</v>
+      </c>
+      <c r="C74" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B75" s="2">
+        <v>74</v>
+      </c>
+      <c r="C75" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B76" s="2">
+        <v>75</v>
+      </c>
+      <c r="C76" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B77" s="2">
+        <v>76</v>
+      </c>
+      <c r="C77" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B78" s="2">
+        <v>77</v>
+      </c>
+      <c r="C78" s="2" t="str">
+        <f t="shared" ref="C78:C89" si="2">SUBSTITUTE(CONCATENATE("local/",A78, ".png"), " ","_")</f>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B79" s="2">
+        <v>78</v>
+      </c>
+      <c r="C79" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B80" s="2">
+        <v>79</v>
+      </c>
+      <c r="C80" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B81" s="2">
+        <v>80</v>
+      </c>
+      <c r="C81" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B82" s="2">
+        <v>81</v>
+      </c>
+      <c r="C82" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B83" s="2">
+        <v>82</v>
+      </c>
+      <c r="C83" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B84" s="2">
+        <v>83</v>
+      </c>
+      <c r="C84" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B85" s="2">
+        <v>84</v>
+      </c>
+      <c r="C85" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B86" s="2">
+        <v>85</v>
+      </c>
+      <c r="C86" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B87" s="2">
+        <v>86</v>
+      </c>
+      <c r="C87" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B88" s="2">
+        <v>87</v>
+      </c>
+      <c r="C88" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="B89" s="2">
+        <v>88</v>
+      </c>
+      <c r="C89" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>local/.png</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Novas imagens adicionadas para projeto
</commit_message>
<xml_diff>
--- a/academia_app/base/treinos.xlsx
+++ b/academia_app/base/treinos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/607c4759856959e0/Documentos/_repositorios_/Projetos/02_academia_app/academia_app/base/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="326" documentId="8_{232220E7-6469-4400-8F27-A04433DD145F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{982979CB-10B7-41C6-99BD-720A21C39FAB}"/>
+  <xr:revisionPtr revIDLastSave="339" documentId="8_{232220E7-6469-4400-8F27-A04433DD145F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56596FAC-A72C-4F95-98AE-F9EFC3FDB104}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{D834B919-9E85-4F8F-893C-9AAA66FB1811}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="52">
   <si>
     <t>Treino A</t>
   </si>
@@ -99,18 +99,12 @@
     <t>Supino Reto com Halter</t>
   </si>
   <si>
-    <t>Supino Inclinado com  Halter</t>
-  </si>
-  <si>
     <t>Crucifixo no Cross Over</t>
   </si>
   <si>
     <t>Peito</t>
   </si>
   <si>
-    <t>Voador_Peck Deck</t>
-  </si>
-  <si>
     <t>Tríceps Corda no Cross Over</t>
   </si>
   <si>
@@ -190,6 +184,15 @@
   </si>
   <si>
     <t>Imagem_Gif</t>
+  </si>
+  <si>
+    <t>Peck Deck</t>
+  </si>
+  <si>
+    <t>Voador</t>
+  </si>
+  <si>
+    <t>Supino Inclinado com Halter</t>
   </si>
 </sst>
 </file>
@@ -250,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -262,7 +265,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,18 +606,18 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="37.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.28515625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="47.140625" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="1" width="11.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="47.140625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -635,14 +637,14 @@
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="4">
@@ -666,7 +668,7 @@
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="4">
@@ -690,7 +692,7 @@
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="4">
@@ -714,7 +716,7 @@
       <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="4">
@@ -738,7 +740,7 @@
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="4">
@@ -762,7 +764,7 @@
       <c r="A7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="4">
@@ -786,7 +788,7 @@
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="4">
@@ -810,7 +812,7 @@
       <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="4">
@@ -834,8 +836,8 @@
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>23</v>
+      <c r="B10" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="C10" s="4">
         <f>VLOOKUP(B10,Base!A:E,2,FALSE)</f>
@@ -843,7 +845,7 @@
       </c>
       <c r="D10" s="4" t="str">
         <f>VLOOKUP(B10,Base!A:E,3,FALSE)</f>
-        <v>local/Imagens/Voador_Peck_Deck.png</v>
+        <v>local/Imagens/Voador.png</v>
       </c>
       <c r="E10" s="4" t="str">
         <f>VLOOKUP(B10,Base!A:E,4,FALSE)</f>
@@ -851,19 +853,19 @@
       </c>
       <c r="F10" s="4" t="str">
         <f>VLOOKUP(B10,Base!A:E,5,FALSE)</f>
-        <v>local/Gifs/Voador_Peck_Deck.gif</v>
+        <v>local/Gifs/Voador.gif</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C11" s="4">
         <f>VLOOKUP(B11,Base!A:E,2,FALSE)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D11" s="4" t="str">
         <f>VLOOKUP(B11,Base!A:E,3,FALSE)</f>
@@ -882,16 +884,16 @@
       <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>20</v>
+      <c r="B12" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="C12" s="4">
         <f>VLOOKUP(B12,Base!A:E,2,FALSE)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D12" s="4" t="str">
         <f>VLOOKUP(B12,Base!A:E,3,FALSE)</f>
-        <v>local/Imagens/Supino_Inclinado_com__Halter.png</v>
+        <v>local/Imagens/Supino_Inclinado_com_Halter.png</v>
       </c>
       <c r="E12" s="4" t="str">
         <f>VLOOKUP(B12,Base!A:E,4,FALSE)</f>
@@ -899,19 +901,19 @@
       </c>
       <c r="F12" s="4" t="str">
         <f>VLOOKUP(B12,Base!A:E,5,FALSE)</f>
-        <v>local/Gifs/Supino_Inclinado_com__Halter.gif</v>
+        <v>local/Gifs/Supino_Inclinado_com_Halter.gif</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>21</v>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C13" s="4">
         <f>VLOOKUP(B13,Base!A:E,2,FALSE)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13" s="4" t="str">
         <f>VLOOKUP(B13,Base!A:E,3,FALSE)</f>
@@ -930,12 +932,12 @@
       <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>25</v>
+      <c r="B14" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="C14" s="4">
         <f>VLOOKUP(B14,Base!A:E,2,FALSE)</f>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D14" s="4" t="str">
         <f>VLOOKUP(B14,Base!A:E,3,FALSE)</f>
@@ -954,12 +956,12 @@
       <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>24</v>
+      <c r="B15" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C15" s="4">
         <f>VLOOKUP(B15,Base!A:E,2,FALSE)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D15" s="4" t="str">
         <f>VLOOKUP(B15,Base!A:E,3,FALSE)</f>
@@ -978,12 +980,12 @@
       <c r="A16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>26</v>
+      <c r="B16" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C16" s="4">
         <f>VLOOKUP(B16,Base!A:E,2,FALSE)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D16" s="4" t="str">
         <f>VLOOKUP(B16,Base!A:E,3,FALSE)</f>
@@ -1002,12 +1004,12 @@
       <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>27</v>
+      <c r="B17" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="C17" s="4">
         <f>VLOOKUP(B17,Base!A:E,2,FALSE)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D17" s="4" t="str">
         <f>VLOOKUP(B17,Base!A:E,3,FALSE)</f>
@@ -1023,15 +1025,15 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>28</v>
+      <c r="A18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C18" s="4">
         <f>VLOOKUP(B18,Base!A:E,2,FALSE)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D18" s="4" t="str">
         <f>VLOOKUP(B18,Base!A:E,3,FALSE)</f>
@@ -1047,15 +1049,15 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>29</v>
+      <c r="A19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="C19" s="4">
         <f>VLOOKUP(B19,Base!A:E,2,FALSE)</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D19" s="4" t="str">
         <f>VLOOKUP(B19,Base!A:E,3,FALSE)</f>
@@ -1071,15 +1073,15 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>30</v>
+      <c r="A20" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="C20" s="4">
         <f>VLOOKUP(B20,Base!A:E,2,FALSE)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D20" s="4" t="str">
         <f>VLOOKUP(B20,Base!A:E,3,FALSE)</f>
@@ -1095,15 +1097,15 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>31</v>
+      <c r="A21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="C21" s="4">
         <f>VLOOKUP(B21,Base!A:E,2,FALSE)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D21" s="4" t="str">
         <f>VLOOKUP(B21,Base!A:E,3,FALSE)</f>
@@ -1119,15 +1121,15 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>32</v>
+      <c r="A22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="C22" s="4">
         <f>VLOOKUP(B22,Base!A:E,2,FALSE)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D22" s="4" t="str">
         <f>VLOOKUP(B22,Base!A:E,3,FALSE)</f>
@@ -1143,15 +1145,15 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>33</v>
+      <c r="A23" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="C23" s="4">
         <f>VLOOKUP(B23,Base!A:E,2,FALSE)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D23" s="4" t="str">
         <f>VLOOKUP(B23,Base!A:E,3,FALSE)</f>
@@ -1167,15 +1169,15 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>34</v>
+      <c r="A24" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="C24" s="4">
         <f>VLOOKUP(B24,Base!A:E,2,FALSE)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D24" s="4" t="str">
         <f>VLOOKUP(B24,Base!A:E,3,FALSE)</f>
@@ -1191,15 +1193,15 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>35</v>
+      <c r="A25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="C25" s="4">
         <f>VLOOKUP(B25,Base!A:E,2,FALSE)</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D25" s="4" t="str">
         <f>VLOOKUP(B25,Base!A:E,3,FALSE)</f>
@@ -1215,15 +1217,15 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>36</v>
+      <c r="A26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="C26" s="4">
         <f>VLOOKUP(B26,Base!A:E,2,FALSE)</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D26" s="4" t="str">
         <f>VLOOKUP(B26,Base!A:E,3,FALSE)</f>
@@ -1239,15 +1241,15 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>37</v>
+      <c r="A27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="C27" s="4">
         <f>VLOOKUP(B27,Base!A:E,2,FALSE)</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D27" s="4" t="str">
         <f>VLOOKUP(B27,Base!A:E,3,FALSE)</f>
@@ -1263,15 +1265,15 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>38</v>
+      <c r="A28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="C28" s="4">
         <f>VLOOKUP(B28,Base!A:E,2,FALSE)</f>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D28" s="4" t="str">
         <f>VLOOKUP(B28,Base!A:E,3,FALSE)</f>
@@ -1287,15 +1289,15 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>39</v>
+      <c r="A29" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="C29" s="4">
         <f>VLOOKUP(B29,Base!A:E,2,FALSE)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D29" s="4" t="str">
         <f>VLOOKUP(B29,Base!A:E,3,FALSE)</f>
@@ -1311,15 +1313,15 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>40</v>
+      <c r="A30" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C30" s="4">
         <f>VLOOKUP(B30,Base!A:E,2,FALSE)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D30" s="4" t="str">
         <f>VLOOKUP(B30,Base!A:E,3,FALSE)</f>
@@ -1335,15 +1337,15 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>49</v>
+      <c r="A31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="C31" s="4">
         <f>VLOOKUP(B31,Base!A:E,2,FALSE)</f>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D31" s="4" t="str">
         <f>VLOOKUP(B31,Base!A:E,3,FALSE)</f>
@@ -1365,7 +1367,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7099EAA6-436F-4116-9FA4-7CBF2CCBFE8A}">
           <x14:formula1>
-            <xm:f>Base!$A$2:$A$31</xm:f>
+            <xm:f>Base!$A$2:$A$32</xm:f>
           </x14:formula1>
           <xm:sqref>B2:B31</xm:sqref>
         </x14:dataValidation>
@@ -1377,11 +1379,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6124B3D7-6BE7-44DE-AAE7-DF9EB59173DA}">
-  <dimension ref="A1:F89"/>
+  <dimension ref="A1:F90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1408,7 +1410,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -1419,7 +1421,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="str">
-        <f t="shared" ref="C2:C66" si="0">SUBSTITUTE(CONCATENATE("local/Imagens/",A2, ".png"), " ","_")</f>
+        <f t="shared" ref="C2:C67" si="0">SUBSTITUTE(CONCATENATE("local/Imagens/",A2, ".png"), " ","_")</f>
         <v>local/Imagens/Pulley_Frente.png</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -1446,7 +1448,7 @@
         <v>5</v>
       </c>
       <c r="E3" s="4" t="str">
-        <f t="shared" ref="E3:E66" si="1">SUBSTITUTE(CONCATENATE("local/Gifs/",A3, ".gif"), " ","_")</f>
+        <f t="shared" ref="E3:E67" si="1">SUBSTITUTE(CONCATENATE("local/Gifs/",A3, ".gif"), " ","_")</f>
         <v>local/Gifs/Remada_Articulada_Pronada.gif</v>
       </c>
     </row>
@@ -1566,433 +1568,439 @@
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="B10" s="4">
         <v>9</v>
       </c>
       <c r="C10" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>local/Imagens/Voador_Peck_Deck.png</v>
+        <v>local/Imagens/Voador.png</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E10" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>local/Gifs/Voador_Peck_Deck.gif</v>
+        <v>local/Gifs/Voador.gif</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="B11" s="4">
         <v>10</v>
       </c>
       <c r="C11" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>local/Imagens/Supino_Reto_com_Halter.png</v>
+        <f t="shared" ref="C11" si="2">SUBSTITUTE(CONCATENATE("local/Imagens/",A11, ".png"), " ","_")</f>
+        <v>local/Imagens/Peck_Deck.png</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E11" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>local/Gifs/Supino_Reto_com_Halter.gif</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" ref="E11" si="3">SUBSTITUTE(CONCATENATE("local/Gifs/",A11, ".gif"), " ","_")</f>
+        <v>local/Gifs/Peck_Deck.gif</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="4">
         <v>11</v>
       </c>
       <c r="C12" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>local/Imagens/Supino_Inclinado_com__Halter.png</v>
+        <v>local/Imagens/Supino_Reto_com_Halter.png</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E12" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>local/Gifs/Supino_Inclinado_com__Halter.gif</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+        <v>local/Gifs/Supino_Reto_com_Halter.gif</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="B13" s="4">
         <v>12</v>
       </c>
       <c r="C13" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>local/Imagens/Crucifixo_no_Cross_Over.png</v>
+        <v>local/Imagens/Supino_Inclinado_com_Halter.png</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>local/Gifs/Crucifixo_no_Cross_Over.gif</v>
+        <v>local/Gifs/Supino_Inclinado_com_Halter.gif</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B14" s="4">
         <v>13</v>
       </c>
       <c r="C14" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>local/Imagens/Tríceps_Francês.png</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>41</v>
+        <v>local/Imagens/Crucifixo_no_Cross_Over.png</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="E14" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>local/Gifs/Tríceps_Francês.gif</v>
+        <v>local/Gifs/Crucifixo_no_Cross_Over.gif</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="4">
         <v>14</v>
       </c>
       <c r="C15" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>local/Imagens/Tríceps_Corda_no_Cross_Over.png</v>
+        <v>local/Imagens/Tríceps_Francês.png</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E15" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>local/Gifs/Tríceps_Corda_no_Cross_Over.gif</v>
+        <v>local/Gifs/Tríceps_Francês.gif</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B16" s="4">
         <v>15</v>
       </c>
       <c r="C16" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>local/Imagens/Tríceps_Unilateral_no_Cross_Over.png</v>
+        <v>local/Imagens/Tríceps_Corda_no_Cross_Over.png</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E16" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>local/Gifs/Tríceps_Unilateral_no_Cross_Over.gif</v>
+        <v>local/Gifs/Tríceps_Corda_no_Cross_Over.gif</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B17" s="4">
         <v>16</v>
       </c>
       <c r="C17" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>local/Imagens/Abdominal_Infra_com_Elevação_de_Pernas.png</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>15</v>
+        <v>local/Imagens/Tríceps_Unilateral_no_Cross_Over.png</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="E17" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>local/Gifs/Abdominal_Infra_com_Elevação_de_Pernas.gif</v>
+        <v>local/Gifs/Tríceps_Unilateral_no_Cross_Over.gif</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B18" s="4">
         <v>17</v>
       </c>
       <c r="C18" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>local/Imagens/Avanço.png</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>42</v>
+        <v>local/Imagens/Abdominal_Infra_com_Elevação_de_Pernas.png</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="E18" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>local/Gifs/Avanço.gif</v>
+        <v>local/Gifs/Abdominal_Infra_com_Elevação_de_Pernas.gif</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B19" s="4">
         <v>18</v>
       </c>
       <c r="C19" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>local/Imagens/Agachamento_Livre.png</v>
+        <v>local/Imagens/Avanço.png</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E19" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>local/Gifs/Agachamento_Livre.gif</v>
+        <v>local/Gifs/Avanço.gif</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B20" s="4">
         <v>19</v>
       </c>
       <c r="C20" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>local/Imagens/Leg_Press_45.png</v>
+        <v>local/Imagens/Agachamento_Livre.png</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E20" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>local/Gifs/Leg_Press_45.gif</v>
+        <v>local/Gifs/Agachamento_Livre.gif</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B21" s="4">
         <v>20</v>
       </c>
       <c r="C21" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>local/Imagens/Cadeira_Extensora.png</v>
+        <v>local/Imagens/Leg_Press_45.png</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E21" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>local/Gifs/Cadeira_Extensora.gif</v>
+        <v>local/Gifs/Leg_Press_45.gif</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B22" s="4">
         <v>21</v>
       </c>
       <c r="C22" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>local/Imagens/Mesa_Flexora.png</v>
+        <v>local/Imagens/Cadeira_Extensora.png</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E22" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>local/Gifs/Mesa_Flexora.gif</v>
+        <v>local/Gifs/Cadeira_Extensora.gif</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B23" s="4">
         <v>22</v>
       </c>
       <c r="C23" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>local/Imagens/Panturrilha_Sentado.png</v>
+        <v>local/Imagens/Mesa_Flexora.png</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E23" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>local/Gifs/Panturrilha_Sentado.gif</v>
+        <v>local/Gifs/Mesa_Flexora.gif</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B24" s="4">
         <v>23</v>
       </c>
       <c r="C24" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>local/Imagens/Abdominal_Supra_Curto.png</v>
+        <v>local/Imagens/Panturrilha_Sentado.png</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>15</v>
+        <v>43</v>
       </c>
       <c r="E24" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>local/Gifs/Abdominal_Supra_Curto.gif</v>
+        <v>local/Gifs/Panturrilha_Sentado.gif</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B25" s="4">
         <v>24</v>
       </c>
       <c r="C25" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>local/Imagens/Remada_Unilateral.png</v>
+        <v>local/Imagens/Abdominal_Supra_Curto.png</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E25" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>local/Gifs/Remada_Unilateral.gif</v>
+        <v>local/Gifs/Abdominal_Supra_Curto.gif</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B26" s="4">
         <v>25</v>
       </c>
       <c r="C26" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>local/Imagens/Remada_Curvada_com_Barra.png</v>
+        <v>local/Imagens/Remada_Unilateral.png</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E26" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>local/Gifs/Remada_Curvada_com_Barra.gif</v>
+        <v>local/Gifs/Remada_Unilateral.gif</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B27" s="4">
         <v>26</v>
       </c>
       <c r="C27" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>local/Imagens/Levantamento_Terra.png</v>
+        <v>local/Imagens/Remada_Curvada_com_Barra.png</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="E27" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>local/Gifs/Levantamento_Terra.gif</v>
+        <v>local/Gifs/Remada_Curvada_com_Barra.gif</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B28" s="4">
         <v>27</v>
       </c>
       <c r="C28" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>local/Imagens/Desenvolvimento_com_Halter.png</v>
+        <v>local/Imagens/Levantamento_Terra.png</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E28" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>local/Gifs/Desenvolvimento_com_Halter.gif</v>
+        <v>local/Gifs/Levantamento_Terra.gif</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B29" s="4">
         <v>28</v>
       </c>
       <c r="C29" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>local/Imagens/Elevação_Lateral_e_Frontal.png</v>
+        <v>local/Imagens/Desenvolvimento_com_Halter.png</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E29" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>local/Gifs/Elevação_Lateral_e_Frontal.gif</v>
+        <v>local/Gifs/Desenvolvimento_com_Halter.gif</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B30" s="4">
         <v>29</v>
       </c>
       <c r="C30" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>local/Imagens/Crucifixo_Inverso_no_Cross_Over.png</v>
+        <v>local/Imagens/Elevação_Lateral_e_Frontal.png</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="E30" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>local/Gifs/Crucifixo_Inverso_no_Cross_Over.gif</v>
+        <v>local/Gifs/Elevação_Lateral_e_Frontal.gif</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="B31" s="4">
         <v>30</v>
       </c>
       <c r="C31" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>local/Imagens/Abdominal_Prancha.png</v>
+        <v>local/Imagens/Crucifixo_Inverso_no_Cross_Over.png</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E31" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>local/Gifs/Abdominal_Prancha.gif</v>
+        <v>local/Gifs/Crucifixo_Inverso_no_Cross_Over.gif</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="B32" s="4">
         <v>31</v>
       </c>
       <c r="C32" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>local/Imagens/.png</v>
+        <v>local/Imagens/Abdominal_Prancha.png</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="E32" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>local/Gifs/.gif</v>
+        <v>local/Gifs/Abdominal_Prancha.gif</v>
       </c>
     </row>
     <row r="33" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -2442,11 +2450,11 @@
         <v>66</v>
       </c>
       <c r="C67" s="4" t="str">
-        <f t="shared" ref="C67:C89" si="2">SUBSTITUTE(CONCATENATE("local/Imagens/",A67, ".png"), " ","_")</f>
+        <f t="shared" si="0"/>
         <v>local/Imagens/.png</v>
       </c>
       <c r="E67" s="4" t="str">
-        <f t="shared" ref="E67:E89" si="3">SUBSTITUTE(CONCATENATE("local/Gifs/",A67, ".gif"), " ","_")</f>
+        <f t="shared" si="1"/>
         <v>local/Gifs/.gif</v>
       </c>
     </row>
@@ -2455,11 +2463,11 @@
         <v>67</v>
       </c>
       <c r="C68" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="C68:C90" si="4">SUBSTITUTE(CONCATENATE("local/Imagens/",A68, ".png"), " ","_")</f>
         <v>local/Imagens/.png</v>
       </c>
       <c r="E68" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="E68:E90" si="5">SUBSTITUTE(CONCATENATE("local/Gifs/",A68, ".gif"), " ","_")</f>
         <v>local/Gifs/.gif</v>
       </c>
     </row>
@@ -2468,11 +2476,11 @@
         <v>68</v>
       </c>
       <c r="C69" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>local/Imagens/.png</v>
       </c>
       <c r="E69" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>local/Gifs/.gif</v>
       </c>
     </row>
@@ -2481,11 +2489,11 @@
         <v>69</v>
       </c>
       <c r="C70" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>local/Imagens/.png</v>
       </c>
       <c r="E70" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>local/Gifs/.gif</v>
       </c>
     </row>
@@ -2494,11 +2502,11 @@
         <v>70</v>
       </c>
       <c r="C71" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>local/Imagens/.png</v>
       </c>
       <c r="E71" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>local/Gifs/.gif</v>
       </c>
     </row>
@@ -2507,11 +2515,11 @@
         <v>71</v>
       </c>
       <c r="C72" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>local/Imagens/.png</v>
       </c>
       <c r="E72" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>local/Gifs/.gif</v>
       </c>
     </row>
@@ -2520,11 +2528,11 @@
         <v>72</v>
       </c>
       <c r="C73" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>local/Imagens/.png</v>
       </c>
       <c r="E73" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>local/Gifs/.gif</v>
       </c>
     </row>
@@ -2533,11 +2541,11 @@
         <v>73</v>
       </c>
       <c r="C74" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>local/Imagens/.png</v>
       </c>
       <c r="E74" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>local/Gifs/.gif</v>
       </c>
     </row>
@@ -2546,11 +2554,11 @@
         <v>74</v>
       </c>
       <c r="C75" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>local/Imagens/.png</v>
       </c>
       <c r="E75" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>local/Gifs/.gif</v>
       </c>
     </row>
@@ -2559,11 +2567,11 @@
         <v>75</v>
       </c>
       <c r="C76" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>local/Imagens/.png</v>
       </c>
       <c r="E76" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>local/Gifs/.gif</v>
       </c>
     </row>
@@ -2572,11 +2580,11 @@
         <v>76</v>
       </c>
       <c r="C77" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>local/Imagens/.png</v>
       </c>
       <c r="E77" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>local/Gifs/.gif</v>
       </c>
     </row>
@@ -2585,11 +2593,11 @@
         <v>77</v>
       </c>
       <c r="C78" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>local/Imagens/.png</v>
       </c>
       <c r="E78" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>local/Gifs/.gif</v>
       </c>
     </row>
@@ -2598,11 +2606,11 @@
         <v>78</v>
       </c>
       <c r="C79" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>local/Imagens/.png</v>
       </c>
       <c r="E79" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>local/Gifs/.gif</v>
       </c>
     </row>
@@ -2611,11 +2619,11 @@
         <v>79</v>
       </c>
       <c r="C80" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>local/Imagens/.png</v>
       </c>
       <c r="E80" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>local/Gifs/.gif</v>
       </c>
     </row>
@@ -2624,11 +2632,11 @@
         <v>80</v>
       </c>
       <c r="C81" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>local/Imagens/.png</v>
       </c>
       <c r="E81" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>local/Gifs/.gif</v>
       </c>
     </row>
@@ -2637,11 +2645,11 @@
         <v>81</v>
       </c>
       <c r="C82" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>local/Imagens/.png</v>
       </c>
       <c r="E82" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>local/Gifs/.gif</v>
       </c>
     </row>
@@ -2650,11 +2658,11 @@
         <v>82</v>
       </c>
       <c r="C83" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>local/Imagens/.png</v>
       </c>
       <c r="E83" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>local/Gifs/.gif</v>
       </c>
     </row>
@@ -2663,11 +2671,11 @@
         <v>83</v>
       </c>
       <c r="C84" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>local/Imagens/.png</v>
       </c>
       <c r="E84" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>local/Gifs/.gif</v>
       </c>
     </row>
@@ -2676,11 +2684,11 @@
         <v>84</v>
       </c>
       <c r="C85" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>local/Imagens/.png</v>
       </c>
       <c r="E85" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>local/Gifs/.gif</v>
       </c>
     </row>
@@ -2689,11 +2697,11 @@
         <v>85</v>
       </c>
       <c r="C86" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>local/Imagens/.png</v>
       </c>
       <c r="E86" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>local/Gifs/.gif</v>
       </c>
     </row>
@@ -2702,11 +2710,11 @@
         <v>86</v>
       </c>
       <c r="C87" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>local/Imagens/.png</v>
       </c>
       <c r="E87" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>local/Gifs/.gif</v>
       </c>
     </row>
@@ -2715,11 +2723,11 @@
         <v>87</v>
       </c>
       <c r="C88" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>local/Imagens/.png</v>
       </c>
       <c r="E88" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>local/Gifs/.gif</v>
       </c>
     </row>
@@ -2728,11 +2736,24 @@
         <v>88</v>
       </c>
       <c r="C89" s="4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>local/Imagens/.png</v>
       </c>
       <c r="E89" s="4" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
+        <v>local/Gifs/.gif</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B90" s="4">
+        <v>89</v>
+      </c>
+      <c r="C90" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>local/Imagens/.png</v>
+      </c>
+      <c r="E90" s="4" t="str">
+        <f t="shared" si="5"/>
         <v>local/Gifs/.gif</v>
       </c>
     </row>

</xml_diff>